<commit_message>
Gitignore and import bug fix
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Progs\DIABETES\sc_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDD09F0-53B1-498B-867D-D058CAFDD23A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C52F2121-E212-40C2-A376-355C8DF0C28A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12707" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{BF398841-AC02-4FD2-B5BC-F61BBB882823}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{BF398841-AC02-4FD2-B5BC-F61BBB882823}"/>
   </bookViews>
   <sheets>
     <sheet name="Stats" sheetId="1" r:id="rId1"/>

</xml_diff>